<commit_message>
Document units for Air Density
</commit_message>
<xml_diff>
--- a/Documentation/Column Descriptions/HPDB Column and Table.xlsx
+++ b/Documentation/Column Descriptions/HPDB Column and Table.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1183" uniqueCount="558">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1187" uniqueCount="560">
   <si>
     <t>Name</t>
   </si>
@@ -1740,6 +1740,12 @@
   </si>
   <si>
     <t>Volume of the fluid displaced by the vessel, in m^3.</t>
+  </si>
+  <si>
+    <t>kg/m^3</t>
+  </si>
+  <si>
+    <t>Density of air, calculated from pressure and temperature.</t>
   </si>
 </sst>
 </file>
@@ -1771,7 +1777,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1781,6 +1787,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1797,7 +1809,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1806,6 +1818,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2391,10 +2404,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F350"/>
+  <dimension ref="A1:F351"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A290" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C310" sqref="C310"/>
+    <sheetView tabSelected="1" topLeftCell="A305" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C331" sqref="C331"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6252,22 +6265,26 @@
       <c r="A330" t="s">
         <v>30</v>
       </c>
-      <c r="B330" t="s">
-        <v>382</v>
-      </c>
-      <c r="E330" t="s">
-        <v>519</v>
+      <c r="B330" s="6" t="s">
+        <v>325</v>
+      </c>
+      <c r="C330" s="6" t="s">
+        <v>558</v>
+      </c>
+      <c r="D330" s="6"/>
+      <c r="E330" s="6" t="s">
+        <v>559</v>
       </c>
     </row>
     <row r="331" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B331" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E331" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="332" spans="1:5" x14ac:dyDescent="0.25">
@@ -6275,21 +6292,21 @@
         <v>31</v>
       </c>
       <c r="B332" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E332" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="333" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B333" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E333" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="334" spans="1:5" x14ac:dyDescent="0.25">
@@ -6297,10 +6314,10 @@
         <v>32</v>
       </c>
       <c r="B334" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E334" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="335" spans="1:5" x14ac:dyDescent="0.25">
@@ -6308,10 +6325,10 @@
         <v>32</v>
       </c>
       <c r="B335" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E335" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="336" spans="1:5" x14ac:dyDescent="0.25">
@@ -6319,38 +6336,38 @@
         <v>32</v>
       </c>
       <c r="B336" t="s">
+        <v>387</v>
+      </c>
+      <c r="E336" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="337" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A337" t="s">
+        <v>32</v>
+      </c>
+      <c r="B337" t="s">
         <v>388</v>
       </c>
-      <c r="C336" t="s">
+      <c r="C337" t="s">
         <v>489</v>
       </c>
-      <c r="E336" t="s">
+      <c r="D337"/>
+      <c r="E337" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="337" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A337" s="3" t="s">
+    <row r="338" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A338" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B337" s="3" t="s">
+      <c r="B338" s="3" t="s">
         <v>389</v>
       </c>
-      <c r="E337" s="3" t="s">
+      <c r="C338" s="3"/>
+      <c r="D338" s="3"/>
+      <c r="E338" s="3" t="s">
         <v>551</v>
-      </c>
-    </row>
-    <row r="338" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A338" t="s">
-        <v>32</v>
-      </c>
-      <c r="B338" t="s">
-        <v>390</v>
-      </c>
-      <c r="C338" t="s">
-        <v>427</v>
-      </c>
-      <c r="E338" t="s">
-        <v>526</v>
       </c>
     </row>
     <row r="339" spans="1:5" x14ac:dyDescent="0.25">
@@ -6358,13 +6375,13 @@
         <v>32</v>
       </c>
       <c r="B339" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C339" t="s">
         <v>427</v>
       </c>
       <c r="E339" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="340" spans="1:5" x14ac:dyDescent="0.25">
@@ -6372,13 +6389,13 @@
         <v>32</v>
       </c>
       <c r="B340" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C340" t="s">
         <v>427</v>
       </c>
       <c r="E340" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="341" spans="1:5" x14ac:dyDescent="0.25">
@@ -6386,10 +6403,13 @@
         <v>32</v>
       </c>
       <c r="B341" t="s">
-        <v>393</v>
+        <v>392</v>
+      </c>
+      <c r="C341" t="s">
+        <v>427</v>
       </c>
       <c r="E341" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="342" spans="1:5" x14ac:dyDescent="0.25">
@@ -6397,13 +6417,10 @@
         <v>32</v>
       </c>
       <c r="B342" t="s">
-        <v>394</v>
-      </c>
-      <c r="C342" t="s">
-        <v>427</v>
+        <v>393</v>
       </c>
       <c r="E342" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="343" spans="1:5" x14ac:dyDescent="0.25">
@@ -6411,10 +6428,13 @@
         <v>32</v>
       </c>
       <c r="B343" t="s">
-        <v>395</v>
+        <v>394</v>
+      </c>
+      <c r="C343" t="s">
+        <v>427</v>
       </c>
       <c r="E343" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="344" spans="1:5" x14ac:dyDescent="0.25">
@@ -6422,13 +6442,10 @@
         <v>32</v>
       </c>
       <c r="B344" t="s">
-        <v>396</v>
-      </c>
-      <c r="C344" t="s">
-        <v>427</v>
+        <v>395</v>
       </c>
       <c r="E344" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="345" spans="1:5" x14ac:dyDescent="0.25">
@@ -6436,35 +6453,38 @@
         <v>32</v>
       </c>
       <c r="B345" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C345" t="s">
         <v>427</v>
       </c>
       <c r="E345" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="346" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B346" t="s">
-        <v>398</v>
+        <v>397</v>
+      </c>
+      <c r="C346" t="s">
+        <v>427</v>
       </c>
       <c r="E346" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="347" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B347" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E347" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="348" spans="1:5" x14ac:dyDescent="0.25">
@@ -6472,16 +6492,10 @@
         <v>34</v>
       </c>
       <c r="B348" t="s">
-        <v>400</v>
-      </c>
-      <c r="C348" t="s">
-        <v>493</v>
-      </c>
-      <c r="D348" t="s">
-        <v>547</v>
+        <v>399</v>
       </c>
       <c r="E348" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="349" spans="1:5" x14ac:dyDescent="0.25">
@@ -6489,10 +6503,16 @@
         <v>34</v>
       </c>
       <c r="B349" t="s">
-        <v>401</v>
+        <v>400</v>
+      </c>
+      <c r="C349" t="s">
+        <v>493</v>
+      </c>
+      <c r="D349" t="s">
+        <v>547</v>
       </c>
       <c r="E349" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="350" spans="1:5" x14ac:dyDescent="0.25">
@@ -6500,9 +6520,20 @@
         <v>34</v>
       </c>
       <c r="B350" t="s">
+        <v>401</v>
+      </c>
+      <c r="E350" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="351" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A351" t="s">
+        <v>34</v>
+      </c>
+      <c r="B351" t="s">
         <v>402</v>
       </c>
-      <c r="E350" t="s">
+      <c r="E351" t="s">
         <v>538</v>
       </c>
     </row>

</xml_diff>